<commit_message>
changed folder names, started bom
</commit_message>
<xml_diff>
--- a/Documents/OMNIXIE.xlsx
+++ b/Documents/OMNIXIE.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21nic\OneDrive\Desktop\NIXIE\OMNIXIE\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21nic\OneDrive\Desktop\NIXIE\OMNIXIE\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD2271B-DE83-4B59-8F09-87D402A1AAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823886F0-014A-4EA9-9536-A5D7F09EDDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CH32V003F4U6 PIN FUNCTIONS" sheetId="1" r:id="rId1"/>
-    <sheet name="PCB MANUFACTURE" sheetId="3" r:id="rId2"/>
+    <sheet name="BOM" sheetId="4" r:id="rId1"/>
+    <sheet name="CH32V003F4U6 PIN FUNCTIONS" sheetId="1" r:id="rId2"/>
+    <sheet name="COST ESTIMATES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
   <si>
     <t>A: ADC, A7 (ADC_IN7)</t>
   </si>
@@ -313,6 +314,147 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>ICs/Modules</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>PI4IOE5V6416ZDEX</t>
+  </si>
+  <si>
+    <t>CH32V003F4U6</t>
+  </si>
+  <si>
+    <t>XC6206P332MR</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>SM04B-SRSS-TB</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount, Right Angle 4 position 0.039" (1.00mm)</t>
+  </si>
+  <si>
+    <t>USB Connectors USB Type C,2.0, Rec,SMT, 0.95mmTH Shell Stakes,G/F,RA,Top Mnt,T&amp;R</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 200MA SOT23</t>
+  </si>
+  <si>
+    <t>QingKe V2 Microprocessor</t>
+  </si>
+  <si>
+    <t>I/O Expander 16 I2C 400 kHz 24-TQFN (4x4)</t>
+  </si>
+  <si>
+    <t>Ref Des</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Plugs &amp; Test Jacks TEST POINT RED .063 </t>
+  </si>
+  <si>
+    <t>Buy bulk from Adafruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPN50R1K4CEATMA1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSS131H6327XTSA1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFETs N-Ch 240V 100mA SOT-23-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATB322515-0110 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK0971114D0B </t>
+  </si>
+  <si>
+    <t>GAN190-650FBEZ</t>
+  </si>
+  <si>
+    <t>770004-4</t>
+  </si>
+  <si>
+    <t>02-09-1104</t>
+  </si>
+  <si>
+    <t>IL-WX-16S-VF-B-E1000E</t>
+  </si>
+  <si>
+    <t>IL-WX-16PB-VF-B-E1000E</t>
+  </si>
+  <si>
+    <t>ATB3225-75011CT-T001</t>
+  </si>
+  <si>
+    <t>SK3200AFL-TP</t>
+  </si>
+  <si>
+    <t>1812B105K251CT</t>
+  </si>
+  <si>
+    <t>Potentiometers Flat 15mm 10k</t>
+  </si>
+  <si>
+    <t>Audio Transformers / Signal Transformers Photoflash Capacitor Charging Transforme</t>
+  </si>
+  <si>
+    <t>GaN FETs SOT8075 650V 11.5A FET</t>
+  </si>
+  <si>
+    <t>Coin Cell Battery Holders COIN CELL HOLDER 12MM</t>
+  </si>
+  <si>
+    <t>MOSFETs CONSUMER</t>
+  </si>
+  <si>
+    <t>Pin &amp; Socket Connectors SOCKET CONTACT</t>
+  </si>
+  <si>
+    <t>Board to Board &amp; Mezzanine Connectors 16POS 0.8MM SMT</t>
+  </si>
+  <si>
+    <t>Board to Board &amp; Mezzanine Connectors 0.8 mm pitch, SMT, parallel/ vertical, 16 pos., Pin header</t>
+  </si>
+  <si>
+    <t>Ferrite Cores &amp; Accessories WE-OEFA LFS Oval Ferrite Core Oval; 25Ohms; 72Ohms Black AEC-Q200</t>
+  </si>
+  <si>
+    <t>Audio Transformers / Signal Transformers 1:1 75ohms 5-200MHz 10dB</t>
+  </si>
+  <si>
+    <t>Schottky Diodes &amp; Rectifiers 3A 200Vr 140Vrms 200V 80A 0.86Vf</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 1812 MLCC X7R 1 uF, +/- 10% 250 V T&amp;R GP</t>
+  </si>
+  <si>
+    <t>Interface - I/O Expanders Interface IO Expander</t>
+  </si>
+  <si>
+    <t>Pin &amp; Socket Connectors CRIMP SKT BULK 14-20</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -322,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,8 +501,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +575,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -688,11 +884,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -793,15 +990,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -810,9 +998,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1237,11 +1475,322 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C7034E-99F6-4C64-9A78-788C06E81851}">
+  <dimension ref="A3:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="56">
+        <v>1</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="54">
+        <v>1</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="54">
+        <v>1</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="50"/>
+    </row>
+    <row r="7" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="54">
+        <v>1</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="59">
+        <v>1</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62">
+        <v>5005</v>
+      </c>
+      <c r="D9" s="62">
+        <v>1</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="64">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="62">
+        <v>2</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="62">
+        <v>1</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="62">
+        <v>1</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="48">
+        <v>1</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="48">
+        <v>12</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="48">
+        <v>1</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="51"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="51"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="48">
+        <v>10</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="48">
+        <v>500</v>
+      </c>
+      <c r="D21" s="48">
+        <v>1</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="48">
+        <v>12</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="48">
+        <v>12</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="48">
+        <v>1</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="48">
+        <v>78201465351</v>
+      </c>
+      <c r="D25" s="48">
+        <v>1</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="48">
+        <v>2</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" display="https://www.mouser.com/ProductDetail/Adafruit/3825?qs=%252BEew9%252B0nqrAn6n76%252BB5vZg%3D%3D" xr:uid="{75C6313B-28DC-4A41-961A-B038562B2C74}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,14 +1812,14 @@
       <c r="E2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
@@ -1763,11 +2312,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC52D2-7558-455D-94BF-A1AB4EDE4282}">
   <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -1781,87 +2330,87 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="40">
         <v>10</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="40">
         <v>5</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="40">
         <v>24.15</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="40">
         <f>SUM(C3:E3)</f>
         <v>39.15</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="40">
         <v>7</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="40">
         <v>2</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <v>42.66</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="40">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="11" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="42" t="s">
         <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="41">
         <v>7.5</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="42" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>